<commit_message>
Updated to newest content
</commit_message>
<xml_diff>
--- a/Documentation/Microprocessor Proposal/Microcontroller Decision Matrix.xlsx
+++ b/Documentation/Microprocessor Proposal/Microcontroller Decision Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Desktop\School\Active Classes\Senior Design\SVN\Documentation\Microprocessor Proposal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Desktop\School\Active Classes\Senior Design\External SVN\Documentation\Microprocessor Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -62,10 +62,10 @@
     <t>Evaluation</t>
   </si>
   <si>
-    <t>C code Programming Ease</t>
-  </si>
-  <si>
     <t>Analog Inputs</t>
+  </si>
+  <si>
+    <t>Programming Ease</t>
   </si>
 </sst>
 </file>
@@ -550,16 +550,20 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -570,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="C1" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D1" s="5">
         <v>0.25</v>
       </c>
       <c r="E1" s="5">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="F1" s="5">
         <v>0.2</v>
@@ -601,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -613,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>11</v>
@@ -625,10 +629,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" s="4">
         <v>5</v>
@@ -644,7 +648,7 @@
       </c>
       <c r="I3" s="6">
         <f>C3*$C$1 +D3*$D$1 + E3*$E$1 + F3*$F$1 + G3*$G$1 + H3*$H$1</f>
-        <v>3.5500000000000003</v>
+        <v>3.8000000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -653,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -672,7 +676,7 @@
       </c>
       <c r="I4" s="6">
         <f t="shared" ref="I4:I6" si="0">C4*$C$1 +D4*$D$1 + E4*$E$1 + F4*$F$1 + G4*$G$1 + H4*$H$1</f>
-        <v>2.85</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -681,10 +685,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="4">
         <v>5</v>
@@ -693,14 +697,14 @@
         <v>3</v>
       </c>
       <c r="G5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -728,7 +732,7 @@
       </c>
       <c r="I6" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>